<commit_message>
manually validated the predictions for batch 1
</commit_message>
<xml_diff>
--- a/validated_batch1.xlsx
+++ b/validated_batch1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gridlock_fer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{591B5615-71B2-4F37-9390-6A01EA96D7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7D8EAB-D596-4EA5-99CB-1469270AD80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3432,8 +3432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A955" workbookViewId="0">
-      <selection activeCell="K996" sqref="K996"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>